<commit_message>
override celltype to string...
</commit_message>
<xml_diff>
--- a/src/main/resources/cross_og_netti.xlsx
+++ b/src/main/resources/cross_og_netti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oles/repos/hm-delbestilling-api/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E70138-3793-7542-89EF-522C5FED9C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622BEFEA-CF5D-2B49-A7FF-482E60391970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-8560" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{93017409-3C97-4F9D-B6EF-863303C7C1B9}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="187">
   <si>
     <t>Deler til kommunale oppdrag Cross 6</t>
   </si>
@@ -598,6 +598,9 @@
   </si>
   <si>
     <t>Netti V sb55</t>
+  </si>
+  <si>
+    <t>220485</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1146,7 @@
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1312,8 +1315,8 @@
       <c r="I5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="7">
-        <v>220485</v>
+      <c r="J5" s="7" t="s">
+        <v>186</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>25</v>
@@ -4109,7 +4112,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="M5:P7 M58:N64 M55:N55 P55 M56:P57 P58:P64 M8:P54 E5:F64 H16:I64 G16:G64 J16:L64 H5:I15 G5:G15 J5:L15" numberStoredAsText="1"/>
+    <ignoredError sqref="M5:P7 M58:N64 M55:N55 P55 M56:P57 P58:P64 M8:P54 E5:F64 H16:I64 G16:G64 J16:L64 H5:I15 G5:G15 J6:L15 K5:L5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>